<commit_message>
Update register allocation logic
</commit_message>
<xml_diff>
--- a/00_Input/02_Emp_Count_Requirement.xlsx
+++ b/00_Input/02_Emp_Count_Requirement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/nich7312_colorado_edu/Documents/01. Study/00. Revision &amp; Self Study/01. Portfolio Projects/04. CU BookStore Scheduling/CU-BookStore-Work-Scheduling/00_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6EFB131-B30F-4DF5-ABC9-2449A7C0A177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{D6EFB131-B30F-4DF5-ABC9-2449A7C0A177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7061EB0-0ED7-4057-B553-D1645186D9CF}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{291D0692-160A-41F9-8A7B-100061AA9CD6}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -666,7 +666,7 @@
         <v>0.3125</v>
       </c>
       <c r="B2" s="12">
-        <f>A2+TIME(0,30,0)</f>
+        <f t="shared" ref="B2:B25" si="0">A2+TIME(0,30,0)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="C2" s="11">
@@ -682,17 +682,17 @@
         <v>0</v>
       </c>
       <c r="G2" s="9">
-        <f>SUM(C2:F2)</f>
+        <f t="shared" ref="G2:G25" si="1">SUM(C2:F2)</f>
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="13">
-        <f>B2</f>
+        <f t="shared" ref="A3:A25" si="2">B2</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="B3" s="12">
-        <f>A3+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.35416666666666663</v>
       </c>
       <c r="C3" s="11">
@@ -712,25 +712,25 @@
         <v>0</v>
       </c>
       <c r="G3" s="9">
-        <f>SUM(C3:F3)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="13">
-        <f>B3</f>
+        <f t="shared" si="2"/>
         <v>0.35416666666666663</v>
       </c>
       <c r="B4" s="12">
-        <f>A4+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.37499999999999994</v>
       </c>
       <c r="C4" s="11">
-        <f>C3</f>
+        <f t="shared" ref="C4:D10" si="3">C3</f>
         <v>3</v>
       </c>
       <c r="D4" s="2">
-        <f>D3</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E4" s="2">
@@ -740,525 +740,525 @@
         <v>1</v>
       </c>
       <c r="G4" s="9">
-        <f>SUM(C4:F4)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="13">
-        <f>B4</f>
+        <f t="shared" si="2"/>
         <v>0.37499999999999994</v>
       </c>
       <c r="B5" s="12">
-        <f>A5+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.39583333333333326</v>
       </c>
       <c r="C5" s="11">
-        <f>C4</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D5" s="2">
-        <f>D4</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E5" s="2">
-        <f>E4</f>
+        <f t="shared" ref="E5:E25" si="4">E4</f>
         <v>1</v>
       </c>
       <c r="F5" s="10">
-        <f>F4</f>
+        <f t="shared" ref="F5:F25" si="5">F4</f>
         <v>1</v>
       </c>
       <c r="G5" s="9">
-        <f>SUM(C5:F5)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="13">
-        <f>B5</f>
+        <f t="shared" si="2"/>
         <v>0.39583333333333326</v>
       </c>
       <c r="B6" s="12">
-        <f>A6+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.41666666666666657</v>
       </c>
       <c r="C6" s="11">
-        <f>C5</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D6" s="2">
-        <f>D5</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E6" s="2">
-        <f>E5</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F6" s="10">
-        <f>F5</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G6" s="9">
-        <f>SUM(C6:F6)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="13">
-        <f>B6</f>
+        <f t="shared" si="2"/>
         <v>0.41666666666666657</v>
       </c>
       <c r="B7" s="12">
-        <f>A7+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.43749999999999989</v>
       </c>
       <c r="C7" s="11">
-        <f>C6</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D7" s="2">
-        <f>D6</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E7" s="2">
-        <f>E6</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F7" s="10">
-        <f>F6</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G7" s="9">
-        <f>SUM(C7:F7)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="13">
-        <f>B7</f>
+        <f t="shared" si="2"/>
         <v>0.43749999999999989</v>
       </c>
       <c r="B8" s="12">
-        <f>A8+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.4583333333333332</v>
       </c>
       <c r="C8" s="11">
-        <f>C7</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D8" s="2">
-        <f>D7</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E8" s="2">
-        <f>E7</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F8" s="10">
-        <f>F7</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G8" s="9">
-        <f>SUM(C8:F8)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="13">
-        <f>B8</f>
+        <f t="shared" si="2"/>
         <v>0.4583333333333332</v>
       </c>
       <c r="B9" s="12">
-        <f>A9+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.47916666666666652</v>
       </c>
       <c r="C9" s="11">
-        <f>C8</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D9" s="2">
-        <f>D8</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E9" s="2">
-        <f>E8</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F9" s="10">
-        <f>F8</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G9" s="9">
-        <f>SUM(C9:F9)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="13">
-        <f>B9</f>
+        <f t="shared" si="2"/>
         <v>0.47916666666666652</v>
       </c>
       <c r="B10" s="12">
-        <f>A10+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.49999999999999983</v>
       </c>
       <c r="C10" s="11">
-        <f>C9</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D10" s="2">
-        <f>D9</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E10" s="2">
-        <f>E9</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F10" s="10">
-        <f>F9</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G10" s="9">
-        <f>SUM(C10:F10)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="13">
-        <f>B10</f>
+        <f t="shared" si="2"/>
         <v>0.49999999999999983</v>
       </c>
       <c r="B11" s="12">
-        <f>A11+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.52083333333333315</v>
       </c>
       <c r="C11" s="11">
         <v>5</v>
       </c>
       <c r="D11" s="2">
-        <f>D10</f>
+        <f t="shared" ref="D11:D25" si="6">D10</f>
         <v>3</v>
       </c>
       <c r="E11" s="2">
-        <f>E10</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F11" s="10">
-        <f>F10</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G11" s="9">
-        <f>SUM(C11:F11)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="13">
-        <f>B11</f>
+        <f t="shared" si="2"/>
         <v>0.52083333333333315</v>
       </c>
       <c r="B12" s="12">
-        <f>A12+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.54166666666666652</v>
       </c>
       <c r="C12" s="11">
-        <f>C11</f>
+        <f t="shared" ref="C12:C20" si="7">C11</f>
         <v>5</v>
       </c>
       <c r="D12" s="2">
-        <f>D11</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E12" s="2">
-        <f>E11</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F12" s="10">
-        <f>F11</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G12" s="9">
-        <f>SUM(C12:F12)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="13">
-        <f>B12</f>
+        <f t="shared" si="2"/>
         <v>0.54166666666666652</v>
       </c>
       <c r="B13" s="12">
-        <f>A13+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.56249999999999989</v>
       </c>
       <c r="C13" s="11">
-        <f>C12</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D13" s="2">
-        <f>D12</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E13" s="2">
-        <f>E12</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F13" s="10">
-        <f>F12</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G13" s="9">
-        <f>SUM(C13:F13)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="13">
-        <f>B13</f>
+        <f t="shared" si="2"/>
         <v>0.56249999999999989</v>
       </c>
       <c r="B14" s="12">
-        <f>A14+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.58333333333333326</v>
       </c>
       <c r="C14" s="11">
-        <f>C13</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D14" s="2">
-        <f>D13</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E14" s="2">
-        <f>E13</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F14" s="10">
-        <f>F13</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G14" s="9">
-        <f>SUM(C14:F14)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="13">
-        <f>B14</f>
+        <f t="shared" si="2"/>
         <v>0.58333333333333326</v>
       </c>
       <c r="B15" s="12">
-        <f>A15+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.60416666666666663</v>
       </c>
       <c r="C15" s="11">
-        <f>C14</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D15" s="2">
-        <f>D14</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E15" s="2">
-        <f>E14</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F15" s="10">
-        <f>F14</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G15" s="9">
-        <f>SUM(C15:F15)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="13">
-        <f>B15</f>
+        <f t="shared" si="2"/>
         <v>0.60416666666666663</v>
       </c>
       <c r="B16" s="12">
-        <f>A16+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.625</v>
       </c>
       <c r="C16" s="11">
-        <f>C15</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D16" s="2">
-        <f>D15</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E16" s="2">
-        <f>E15</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F16" s="10">
-        <f>F15</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G16" s="9">
-        <f>SUM(C16:F16)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="13">
-        <f>B16</f>
+        <f t="shared" si="2"/>
         <v>0.625</v>
       </c>
       <c r="B17" s="12">
-        <f>A17+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.64583333333333337</v>
       </c>
       <c r="C17" s="11">
-        <f>C16</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D17" s="2">
-        <f>D16</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E17" s="2">
-        <f>E16</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F17" s="10">
-        <f>F16</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G17" s="9">
-        <f>SUM(C17:F17)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="13">
-        <f>B17</f>
+        <f t="shared" si="2"/>
         <v>0.64583333333333337</v>
       </c>
       <c r="B18" s="12">
-        <f>A18+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="C18" s="11">
-        <f>C17</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D18" s="2">
-        <f>D17</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E18" s="2">
-        <f>E17</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F18" s="10">
-        <f>F17</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G18" s="9">
-        <f>SUM(C18:F18)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="13">
-        <f>B18</f>
+        <f t="shared" si="2"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="B19" s="12">
-        <f>A19+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.68750000000000011</v>
       </c>
       <c r="C19" s="11">
-        <f>C18</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D19" s="2">
-        <f>D18</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E19" s="2">
-        <f>E18</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F19" s="10">
-        <f>F18</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G19" s="9">
-        <f>SUM(C19:F19)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="13">
-        <f>B19</f>
+        <f t="shared" si="2"/>
         <v>0.68750000000000011</v>
       </c>
       <c r="B20" s="12">
-        <f>A20+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.70833333333333348</v>
       </c>
       <c r="C20" s="11">
-        <f>C19</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D20" s="2">
-        <f>D19</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E20" s="2">
-        <f>E19</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F20" s="10">
-        <f>F19</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G20" s="9">
-        <f>SUM(C20:F20)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="13">
-        <f>B20</f>
+        <f t="shared" si="2"/>
         <v>0.70833333333333348</v>
       </c>
       <c r="B21" s="12">
-        <f>A21+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.72916666666666685</v>
       </c>
       <c r="C21" s="11">
         <v>2</v>
       </c>
       <c r="D21" s="2">
-        <f>D20</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E21" s="2">
-        <f>E20</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F21" s="10">
-        <f>F20</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G21" s="9">
-        <f>SUM(C21:F21)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="13">
-        <f>B21</f>
+        <f t="shared" si="2"/>
         <v>0.72916666666666685</v>
       </c>
       <c r="B22" s="12">
-        <f>A22+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.75000000000000022</v>
       </c>
       <c r="C22" s="11">
@@ -1266,29 +1266,29 @@
         <v>2</v>
       </c>
       <c r="D22" s="2">
-        <f>D21</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E22" s="2">
-        <f>E21</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F22" s="10">
-        <f>F21</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G22" s="9">
-        <f>SUM(C22:F22)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="13">
-        <f>B22</f>
+        <f t="shared" si="2"/>
         <v>0.75000000000000022</v>
       </c>
       <c r="B23" s="12">
-        <f>A23+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.77083333333333359</v>
       </c>
       <c r="C23" s="11">
@@ -1296,29 +1296,29 @@
         <v>2</v>
       </c>
       <c r="D23" s="2">
-        <f>D22</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E23" s="2">
-        <f>E22</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F23" s="10">
-        <f>F22</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G23" s="9">
-        <f>SUM(C23:F23)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="13">
-        <f>B23</f>
+        <f t="shared" si="2"/>
         <v>0.77083333333333359</v>
       </c>
       <c r="B24" s="12">
-        <f>A24+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.79166666666666696</v>
       </c>
       <c r="C24" s="11">
@@ -1326,29 +1326,29 @@
         <v>2</v>
       </c>
       <c r="D24" s="2">
-        <f>D23</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E24" s="2">
-        <f>E23</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F24" s="10">
-        <f>F23</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G24" s="9">
-        <f>SUM(C24:F24)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="8">
-        <f>B24</f>
+        <f t="shared" si="2"/>
         <v>0.79166666666666696</v>
       </c>
       <c r="B25" s="7">
-        <f>A25+TIME(0,30,0)</f>
+        <f t="shared" si="0"/>
         <v>0.81250000000000033</v>
       </c>
       <c r="C25" s="6">
@@ -1356,19 +1356,19 @@
         <v>2</v>
       </c>
       <c r="D25" s="5">
-        <f>D24</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E25" s="5">
-        <f>E24</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F25" s="4">
-        <f>F24</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G25" s="3">
-        <f>SUM(C25:F25)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated with final allocation logic
</commit_message>
<xml_diff>
--- a/00_Input/02_Emp_Count_Requirement.xlsx
+++ b/00_Input/02_Emp_Count_Requirement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/nich7312_colorado_edu/Documents/01. Study/00. Revision &amp; Self Study/01. Portfolio Projects/04. CU BookStore Scheduling/CU-BookStore-Work-Scheduling/00_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{D6EFB131-B30F-4DF5-ABC9-2449A7C0A177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7061EB0-0ED7-4057-B553-D1645186D9CF}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{D6EFB131-B30F-4DF5-ABC9-2449A7C0A177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F837EDF-69A2-4600-92D8-C360D4E1C665}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{291D0692-160A-41F9-8A7B-100061AA9CD6}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -670,10 +670,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C2" s="11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -683,7 +683,7 @@
       </c>
       <c r="G2" s="9">
         <f t="shared" ref="G2:G25" si="1">SUM(C2:F2)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -697,11 +697,11 @@
       </c>
       <c r="C3" s="11">
         <f>C2</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
         <f>D2</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2">
         <f>E2</f>
@@ -713,7 +713,7 @@
       </c>
       <c r="G3" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -727,26 +727,26 @@
       </c>
       <c r="C4" s="11">
         <f t="shared" ref="C4:D10" si="3">C3</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="13">
-        <f t="shared" si="2"/>
+        <f>B4</f>
         <v>0.37499999999999994</v>
       </c>
       <c r="B5" s="12">
@@ -754,24 +754,21 @@
         <v>0.39583333333333326</v>
       </c>
       <c r="C5" s="11">
-        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E25" si="4">E4</f>
         <v>1</v>
       </c>
       <c r="F5" s="10">
-        <f t="shared" ref="F5:F25" si="5">F4</f>
-        <v>1</v>
+        <f>F4</f>
+        <v>0</v>
       </c>
       <c r="G5" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -792,16 +789,16 @@
         <v>3</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E6:E25" si="4">E5</f>
         <v>1</v>
       </c>
       <c r="F6" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" ref="F6:F25" si="5">F5</f>
+        <v>0</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -827,11 +824,11 @@
       </c>
       <c r="F7" s="10">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -857,11 +854,11 @@
       </c>
       <c r="F8" s="10">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -886,7 +883,6 @@
         <v>1</v>
       </c>
       <c r="F9" s="10">
-        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G9" s="9">
@@ -934,7 +930,7 @@
         <v>0.52083333333333315</v>
       </c>
       <c r="C11" s="11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" ref="D11:D25" si="6">D10</f>
@@ -950,7 +946,7 @@
       </c>
       <c r="G11" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -964,7 +960,7 @@
       </c>
       <c r="C12" s="11">
         <f t="shared" ref="C12:C20" si="7">C11</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="6"/>
@@ -980,7 +976,7 @@
       </c>
       <c r="G12" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -994,7 +990,7 @@
       </c>
       <c r="C13" s="11">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="6"/>
@@ -1010,7 +1006,7 @@
       </c>
       <c r="G13" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -1024,7 +1020,7 @@
       </c>
       <c r="C14" s="11">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="6"/>
@@ -1040,7 +1036,7 @@
       </c>
       <c r="G14" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -1054,7 +1050,7 @@
       </c>
       <c r="C15" s="11">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="6"/>
@@ -1070,7 +1066,7 @@
       </c>
       <c r="G15" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -1084,7 +1080,7 @@
       </c>
       <c r="C16" s="11">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="6"/>
@@ -1100,7 +1096,7 @@
       </c>
       <c r="G16" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -1114,7 +1110,7 @@
       </c>
       <c r="C17" s="11">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="6"/>
@@ -1130,7 +1126,7 @@
       </c>
       <c r="G17" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
@@ -1144,7 +1140,7 @@
       </c>
       <c r="C18" s="11">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="6"/>
@@ -1160,7 +1156,7 @@
       </c>
       <c r="G18" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
@@ -1174,7 +1170,7 @@
       </c>
       <c r="C19" s="11">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="6"/>
@@ -1190,7 +1186,7 @@
       </c>
       <c r="G19" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -1204,7 +1200,7 @@
       </c>
       <c r="C20" s="11">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="6"/>
@@ -1220,7 +1216,7 @@
       </c>
       <c r="G20" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -1233,23 +1229,21 @@
         <v>0.72916666666666685</v>
       </c>
       <c r="C21" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F21" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
@@ -1263,11 +1257,11 @@
       </c>
       <c r="C22" s="11">
         <f>C21</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="4"/>
@@ -1275,11 +1269,11 @@
       </c>
       <c r="F22" s="10">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
@@ -1292,24 +1286,20 @@
         <v>0.77083333333333359</v>
       </c>
       <c r="C23" s="11">
-        <f>C22</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
@@ -1323,23 +1313,23 @@
       </c>
       <c r="C24" s="11">
         <f>C23</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="10">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1353,23 +1343,23 @@
       </c>
       <c r="C25" s="6">
         <f>C24</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25" s="5">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E25" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with emp view and SF allocation based on previous up/down shhift
</commit_message>
<xml_diff>
--- a/00_Input/02_Emp_Count_Requirement.xlsx
+++ b/00_Input/02_Emp_Count_Requirement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/nich7312_colorado_edu/Documents/01. Study/00. Revision &amp; Self Study/01. Portfolio Projects/04. CU BookStore Scheduling/CU-BookStore-Work-Scheduling/00_Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/nich7312_colorado_edu/Documents/01. Study/00. Revision &amp; Self Study/01. Portfolio Projects/04. CU BookStore Scheduling/BuffRoSTOREing Working Repo/00_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{D6EFB131-B30F-4DF5-ABC9-2449A7C0A177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F837EDF-69A2-4600-92D8-C360D4E1C665}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{D6EFB131-B30F-4DF5-ABC9-2449A7C0A177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE679138-F470-4B9E-860B-495A1DD876E4}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{291D0692-160A-41F9-8A7B-100061AA9CD6}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -754,13 +754,13 @@
         <v>0.39583333333333326</v>
       </c>
       <c r="C5" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="10">
         <f>F4</f>
@@ -768,7 +768,7 @@
       </c>
       <c r="G5" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -782,23 +782,22 @@
       </c>
       <c r="C6" s="11">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" ref="E6:E25" si="4">E5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="10">
-        <f t="shared" ref="F6:F25" si="5">F5</f>
+        <f t="shared" ref="F6:F25" si="4">F5</f>
         <v>0</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -812,23 +811,21 @@
       </c>
       <c r="C7" s="11">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F7" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -842,23 +839,23 @@
       </c>
       <c r="C8" s="11">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="2">
+        <f t="shared" ref="E8:E25" si="5">E7</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F8" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="G8" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -872,14 +869,14 @@
       </c>
       <c r="C9" s="11">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F9" s="10">
@@ -887,7 +884,7 @@
       </c>
       <c r="G9" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -901,23 +898,23 @@
       </c>
       <c r="C10" s="11">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F10" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="G10" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
@@ -930,23 +927,23 @@
         <v>0.52083333333333315</v>
       </c>
       <c r="C11" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" ref="D11:D25" si="6">D10</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F11" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="G11" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -960,23 +957,23 @@
       </c>
       <c r="C12" s="11">
         <f t="shared" ref="C12:C20" si="7">C11</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F12" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="G12" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -990,23 +987,23 @@
       </c>
       <c r="C13" s="11">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F13" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="G13" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -1020,23 +1017,23 @@
       </c>
       <c r="C14" s="11">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F14" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F14" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="G14" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -1050,23 +1047,23 @@
       </c>
       <c r="C15" s="11">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F15" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="G15" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -1080,23 +1077,23 @@
       </c>
       <c r="C16" s="11">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F16" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="G16" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -1110,23 +1107,23 @@
       </c>
       <c r="C17" s="11">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F17" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F17" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="G17" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
@@ -1140,23 +1137,23 @@
       </c>
       <c r="C18" s="11">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F18" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F18" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="G18" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
@@ -1170,23 +1167,23 @@
       </c>
       <c r="C19" s="11">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F19" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F19" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="G19" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -1200,23 +1197,23 @@
       </c>
       <c r="C20" s="11">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F20" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F20" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="G20" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -1229,21 +1226,21 @@
         <v>0.72916666666666685</v>
       </c>
       <c r="C21" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F21" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
@@ -1257,23 +1254,22 @@
       </c>
       <c r="C22" s="11">
         <f>C21</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E22" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F22" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F22" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="G22" s="9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
@@ -1320,11 +1316,11 @@
         <v>0</v>
       </c>
       <c r="E24" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="10">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G24" s="9">
@@ -1350,11 +1346,11 @@
         <v>0</v>
       </c>
       <c r="E25" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="4">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G25" s="3">

</xml_diff>